<commit_message>
Commit of reworked frontend.
</commit_message>
<xml_diff>
--- a/api/scraper/global_oc_index.xlsx
+++ b/api/scraper/global_oc_index.xlsx
@@ -145,7 +145,7 @@
     <t>Somalia</t>
   </si>
   <si>
-    <t>Korea, DPR</t>
+    <t>North Korea</t>
   </si>
   <si>
     <t>Venezuela</t>
@@ -691,7 +691,7 @@
     <t>Andorra</t>
   </si>
   <si>
-    <t>Korea, Rep,</t>
+    <t>South Korea</t>
   </si>
   <si>
     <t>Denmark</t>
@@ -765,7 +765,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2927,7 +2927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18">
       <c r="A17" s="1" t="s">
         <v>52</v>
       </c>
@@ -3040,7 +3040,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18">
       <c r="A18" s="1" t="s">
         <v>53</v>
       </c>
@@ -3153,7 +3153,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18">
       <c r="A19" s="1" t="s">
         <v>54</v>
       </c>
@@ -3266,7 +3266,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18">
       <c r="A20" s="1" t="s">
         <v>55</v>
       </c>
@@ -3379,7 +3379,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18">
       <c r="A21" s="1" t="s">
         <v>56</v>
       </c>
@@ -3492,7 +3492,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18">
       <c r="A22" s="1" t="s">
         <v>57</v>
       </c>
@@ -3605,7 +3605,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18">
       <c r="A23" s="1" t="s">
         <v>58</v>
       </c>
@@ -3718,7 +3718,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18">
       <c r="A24" s="1" t="s">
         <v>59</v>
       </c>
@@ -3831,7 +3831,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18">
       <c r="A25" s="1" t="s">
         <v>60</v>
       </c>
@@ -3944,7 +3944,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18">
       <c r="A26" s="1" t="s">
         <v>61</v>
       </c>

</xml_diff>